<commit_message>
adds readings to syllabus
</commit_message>
<xml_diff>
--- a/syllabus/330-syllabus.xlsx
+++ b/syllabus/330-syllabus.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="154">
   <si>
     <t>Lecture</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Physics of Energy</t>
   </si>
   <si>
-    <t>Biological Processes</t>
-  </si>
-  <si>
     <t>Energy Conversion</t>
   </si>
   <si>
@@ -153,12 +150,6 @@
     <t>Energy Efficiency</t>
   </si>
   <si>
-    <t>Climate Impacts of Energy</t>
-  </si>
-  <si>
-    <t>Health Impacts of Energy</t>
-  </si>
-  <si>
     <t>Global Access to Energy</t>
   </si>
   <si>
@@ -180,15 +171,9 @@
     <t>Homework Reflection 3</t>
   </si>
   <si>
-    <t>Timeline</t>
-  </si>
-  <si>
     <t>Wrapup</t>
   </si>
   <si>
-    <t>Local/global Energy Solutions</t>
-  </si>
-  <si>
     <t>Presentations</t>
   </si>
   <si>
@@ -291,12 +276,6 @@
     <t>Lovins 1976</t>
   </si>
   <si>
-    <t>NC-12</t>
-  </si>
-  <si>
-    <t>NC-14</t>
-  </si>
-  <si>
     <t>Toolkit 1</t>
   </si>
   <si>
@@ -324,21 +303,12 @@
     <t>Policy</t>
   </si>
   <si>
-    <t>Solutions</t>
-  </si>
-  <si>
     <t>Projects</t>
   </si>
   <si>
     <t>HK-13 The Building Blocks of Matter, HK-14 Nuclear Power Fission, Moore 2005</t>
   </si>
   <si>
-    <t>HK-07 Energy from fossil fuels, HK-08 Air Pollution and Energy Use</t>
-  </si>
-  <si>
-    <t>masters?</t>
-  </si>
-  <si>
     <t>fracking?</t>
   </si>
   <si>
@@ -348,15 +318,6 @@
     <t>Life Cycle Energy and Cost Analysis</t>
   </si>
   <si>
-    <t>Water and Drought</t>
-  </si>
-  <si>
-    <t>Hydraulic Fracturing</t>
-  </si>
-  <si>
-    <t>Water-Energy Nexus</t>
-  </si>
-  <si>
     <t>Activity</t>
   </si>
   <si>
@@ -384,15 +345,9 @@
     <t>Climate negotiation discussion</t>
   </si>
   <si>
-    <t>Economics module</t>
-  </si>
-  <si>
     <t>Carol Dweck, Mindset</t>
   </si>
   <si>
-    <t>HK-01, HK-02</t>
-  </si>
-  <si>
     <t>REPL Calculations</t>
   </si>
   <si>
@@ -423,27 +378,15 @@
     <t>Last Year Reading</t>
   </si>
   <si>
-    <t>Masters 4.1 4.2</t>
-  </si>
-  <si>
     <t>Nat Cap Ch 10, hot air 13</t>
   </si>
   <si>
     <t>Masters 1991 energy</t>
   </si>
   <si>
-    <t>H&amp;K 7&amp;8</t>
-  </si>
-  <si>
     <t>Masters ch 1</t>
   </si>
   <si>
-    <t>H&amp;K 13 &amp; 14</t>
-  </si>
-  <si>
-    <t>M&amp;R Ch 5</t>
-  </si>
-  <si>
     <t>Moore</t>
   </si>
   <si>
@@ -462,23 +405,94 @@
     <t>Wedges, safe operating space?</t>
   </si>
   <si>
-    <t>HK-03, HK-04</t>
-  </si>
-  <si>
     <t>GMC Sustainability Day</t>
+  </si>
+  <si>
+    <t>rational middle videos</t>
+  </si>
+  <si>
+    <t>Carbon (Critters and Combustion)</t>
+  </si>
+  <si>
+    <t>Mackay-07 Heating and Cooling</t>
+  </si>
+  <si>
+    <t>Mackay-01, HK-01-Introduction, HK-02-Energy Mechanics</t>
+  </si>
+  <si>
+    <t>HK-03-Conservation of Energy, HK-04-Heat and Work</t>
+  </si>
+  <si>
+    <t>HK-07 Energy from Fossil Fuels</t>
+  </si>
+  <si>
+    <t>HK-08 Air Pollution and Energy Use</t>
+  </si>
+  <si>
+    <t>HK-09 Global Warming and Thermal Pollution</t>
+  </si>
+  <si>
+    <t>HK-19 A National and Personal Commitment</t>
+  </si>
+  <si>
+    <t>NC-11 Aqueous Solutions</t>
+  </si>
+  <si>
+    <t>NC-12 Climate</t>
+  </si>
+  <si>
+    <t>NC-14 Human Capitalism</t>
+  </si>
+  <si>
+    <t>Energy and Water</t>
+  </si>
+  <si>
+    <t>Energy and Agriculture</t>
+  </si>
+  <si>
+    <t>Energy and Human Health</t>
+  </si>
+  <si>
+    <t>Energy and Climate</t>
+  </si>
+  <si>
+    <t>Mackay-03 Cars, NC-02 Reinventing the Wheels</t>
+  </si>
+  <si>
+    <t>NC-12 Climate, NC-14 Human Capitalism</t>
+  </si>
+  <si>
+    <t>Energy and Economics</t>
+  </si>
+  <si>
+    <t>TBD (Randolph and Masters?)</t>
+  </si>
+  <si>
+    <t>NC-11 Aqueous Solutions, EPA Hydraulic Fracturing Study</t>
+  </si>
+  <si>
+    <t>Pacala and Socolow Wedges</t>
+  </si>
+  <si>
+    <t>NAACP Coal Blooded</t>
+  </si>
+  <si>
+    <t>Mackay-13 Food and farming, NC-10 Food for Life</t>
+  </si>
+  <si>
+    <t>Power Africa Report, Goldemberg 1985</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -517,6 +531,14 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -535,7 +557,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="107">
+  <cellStyleXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -643,8 +665,66 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -675,8 +755,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="107">
+  <cellStyles count="165">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -730,6 +820,35 @@
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -783,6 +902,35 @@
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1115,10 +1263,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1127,17 +1275,18 @@
     <col min="2" max="2" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="65.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="70.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="25.1640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="65.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="18" customHeight="1">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -1150,33 +1299,36 @@
       <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>112</v>
+      <c r="E1" s="12" t="s">
+        <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1"/>
-      <c r="L1" s="10" t="s">
-        <v>95</v>
-      </c>
+      <c r="L1"/>
       <c r="M1" s="10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>88</v>
+      </c>
+      <c r="N1" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1184,25 +1336,24 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="5"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="6"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
-      <c r="K2"/>
-      <c r="L2" t="s">
-        <v>96</v>
-      </c>
+      <c r="J2" s="5"/>
+      <c r="L2"/>
       <c r="M2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>89</v>
+      </c>
+      <c r="N2"/>
+    </row>
+    <row r="3" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1210,34 +1361,34 @@
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5" t="s">
+      <c r="E3" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="K3"/>
-      <c r="L3" t="s">
-        <v>96</v>
-      </c>
-      <c r="M3" s="9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="J3" s="5"/>
+      <c r="K3" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="L3"/>
+      <c r="M3" t="s">
+        <v>89</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -1245,30 +1396,34 @@
         <v>3</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="6"/>
-      <c r="F4" s="5"/>
+      <c r="E4" s="14" t="s">
+        <v>85</v>
+      </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="K4"/>
-      <c r="L4" t="s">
-        <v>96</v>
-      </c>
-      <c r="M4" s="9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>8</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="L4"/>
+      <c r="M4" t="s">
+        <v>89</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -1276,30 +1431,30 @@
         <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>125</v>
-      </c>
-      <c r="F5" s="5"/>
+      <c r="E5" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>110</v>
+      </c>
       <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="K5"/>
-      <c r="L5" t="s">
-        <v>96</v>
-      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="L5"/>
       <c r="M5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="N5"/>
+    </row>
+    <row r="6" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -1307,30 +1462,30 @@
         <v>5</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F6" s="5"/>
+      <c r="E6" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>102</v>
+      </c>
       <c r="G6" s="5"/>
-      <c r="H6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="5"/>
-      <c r="J6" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="K6"/>
-      <c r="L6" t="s">
-        <v>96</v>
-      </c>
-      <c r="M6"/>
-    </row>
-    <row r="7" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="H6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="L6"/>
+      <c r="M6" t="s">
+        <v>89</v>
+      </c>
+      <c r="N6"/>
+    </row>
+    <row r="7" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -1338,29 +1493,35 @@
         <v>6</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="7"/>
-      <c r="I7" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="K7"/>
-      <c r="L7" t="s">
-        <v>96</v>
-      </c>
-      <c r="M7"/>
-    </row>
-    <row r="8" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="I7" s="7"/>
+      <c r="J7" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="L7"/>
+      <c r="M7" t="s">
+        <v>89</v>
+      </c>
+      <c r="N7"/>
+    </row>
+    <row r="8" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -1368,30 +1529,31 @@
         <v>7</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="6"/>
-      <c r="F8" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="6"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="K8"/>
-      <c r="L8" t="s">
-        <v>97</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="H8" s="5"/>
+      <c r="I8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="L8"/>
+      <c r="M8" t="s">
+        <v>90</v>
+      </c>
+      <c r="N8" s="11"/>
+    </row>
+    <row r="9" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="5">
         <v>4</v>
       </c>
@@ -1399,30 +1561,33 @@
         <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="5"/>
+        <v>98</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5" t="s">
+        <v>47</v>
+      </c>
       <c r="I9" s="5"/>
-      <c r="J9" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="K9"/>
-      <c r="L9" t="s">
-        <v>97</v>
-      </c>
-      <c r="M9"/>
-    </row>
-    <row r="10" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="J9" s="5"/>
+      <c r="K9" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="L9"/>
+      <c r="M9" t="s">
+        <v>90</v>
+      </c>
+      <c r="N9"/>
+    </row>
+    <row r="10" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A10" s="5">
         <v>5</v>
       </c>
@@ -1430,32 +1595,35 @@
         <v>9</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="J10" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="K10"/>
-      <c r="L10" t="s">
-        <v>97</v>
-      </c>
-      <c r="M10" s="9" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>147</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="L10"/>
+      <c r="M10" t="s">
+        <v>90</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A11" s="5">
         <v>5</v>
       </c>
@@ -1463,29 +1631,30 @@
         <v>10</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="5"/>
-      <c r="K11"/>
-      <c r="L11" t="s">
-        <v>97</v>
-      </c>
+      <c r="J11" s="5"/>
+      <c r="L11"/>
       <c r="M11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>90</v>
+      </c>
+      <c r="N11"/>
+    </row>
+    <row r="12" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A12" s="5">
         <v>6</v>
       </c>
@@ -1493,27 +1662,28 @@
         <v>11</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>33</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-      <c r="K12"/>
-      <c r="L12" t="s">
-        <v>97</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="J12" s="5"/>
+      <c r="L12"/>
+      <c r="M12" t="s">
+        <v>90</v>
+      </c>
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A13" s="5">
         <v>6</v>
       </c>
@@ -1521,29 +1691,29 @@
         <v>12</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="6"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H13" s="7"/>
-      <c r="I13" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="K13"/>
-      <c r="L13" t="s">
-        <v>97</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L13"/>
       <c r="M13" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>90</v>
+      </c>
+      <c r="N13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A14" s="5">
         <v>7</v>
       </c>
@@ -1551,30 +1721,30 @@
         <v>13</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="F14" s="5"/>
+        <v>35</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>100</v>
+      </c>
       <c r="G14" s="5"/>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="5"/>
+      <c r="I14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="K14"/>
-      <c r="L14" t="s">
-        <v>97</v>
-      </c>
-      <c r="M14"/>
-    </row>
-    <row r="15" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="J14" s="5"/>
+      <c r="K14" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="L14"/>
+      <c r="M14" t="s">
+        <v>90</v>
+      </c>
+      <c r="N14"/>
+    </row>
+    <row r="15" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A15" s="5">
         <v>7</v>
       </c>
@@ -1582,26 +1752,27 @@
         <v>14</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15" s="6"/>
-      <c r="F15" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="F15" s="6"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="9" t="s">
-        <v>105</v>
-      </c>
-      <c r="K15"/>
-      <c r="L15" t="s">
-        <v>98</v>
-      </c>
-      <c r="M15"/>
-    </row>
-    <row r="16" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="H15" s="5"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="9"/>
+      <c r="L15"/>
+      <c r="M15" t="s">
+        <v>91</v>
+      </c>
+      <c r="N15"/>
+    </row>
+    <row r="16" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A16" s="5">
         <v>8</v>
       </c>
@@ -1609,28 +1780,30 @@
         <v>15</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="J16" s="9"/>
-      <c r="K16"/>
-      <c r="L16" t="s">
-        <v>98</v>
-      </c>
-      <c r="M16"/>
-    </row>
-    <row r="17" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="I16" s="5"/>
+      <c r="J16" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="K16" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="L16"/>
+      <c r="M16" t="s">
+        <v>91</v>
+      </c>
+      <c r="N16"/>
+    </row>
+    <row r="17" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A17" s="5">
         <v>8</v>
       </c>
@@ -1638,28 +1811,30 @@
         <v>16</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="F17" s="6"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="5"/>
+      <c r="I17" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I17" s="5"/>
-      <c r="J17" s="9"/>
-      <c r="K17" t="s">
-        <v>88</v>
-      </c>
+      <c r="J17" s="5"/>
       <c r="L17" t="s">
-        <v>98</v>
-      </c>
-      <c r="M17"/>
-    </row>
-    <row r="18" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>83</v>
+      </c>
+      <c r="M17" t="s">
+        <v>91</v>
+      </c>
+      <c r="N17"/>
+    </row>
+    <row r="18" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A18" s="5">
         <v>9</v>
       </c>
@@ -1667,28 +1842,29 @@
         <v>17</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H18" s="7"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="9"/>
-      <c r="K18" t="s">
-        <v>88</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="9"/>
       <c r="L18" t="s">
-        <v>98</v>
-      </c>
-      <c r="M18"/>
-    </row>
-    <row r="19" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>83</v>
+      </c>
+      <c r="M18" t="s">
+        <v>91</v>
+      </c>
+      <c r="N18"/>
+    </row>
+    <row r="19" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A19" s="5">
         <v>9</v>
       </c>
@@ -1696,26 +1872,26 @@
         <v>18</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="5"/>
+        <v>40</v>
+      </c>
+      <c r="F19" s="6"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
-      <c r="I19" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="J19" s="9"/>
-      <c r="K19"/>
-      <c r="L19" t="s">
-        <v>98</v>
-      </c>
-      <c r="M19"/>
-    </row>
-    <row r="20" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="I19" s="5"/>
+      <c r="J19" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="K19" s="9"/>
+      <c r="L19"/>
+      <c r="M19" t="s">
+        <v>91</v>
+      </c>
+      <c r="N19"/>
+    </row>
+    <row r="20" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A20" s="5">
         <v>10</v>
       </c>
@@ -1723,32 +1899,33 @@
         <v>19</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="14"/>
+      <c r="F20" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="I20" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I20" s="5"/>
-      <c r="J20" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="K20"/>
-      <c r="L20" t="s">
-        <v>99</v>
-      </c>
-      <c r="M20"/>
-    </row>
-    <row r="21" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="J20" s="5"/>
+      <c r="K20" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="L20"/>
+      <c r="M20" t="s">
+        <v>92</v>
+      </c>
+      <c r="N20"/>
+    </row>
+    <row r="21" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A21" s="5">
         <v>10</v>
       </c>
@@ -1756,24 +1933,29 @@
         <v>20</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="6"/>
-      <c r="F21" s="5"/>
+        <v>42</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="F21" s="6"/>
       <c r="G21" s="5"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="9"/>
-      <c r="K21"/>
-      <c r="L21" t="s">
-        <v>99</v>
-      </c>
-      <c r="M21"/>
-    </row>
-    <row r="22" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="H21" s="5"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="L21"/>
+      <c r="M21" t="s">
+        <v>92</v>
+      </c>
+      <c r="N21"/>
+    </row>
+    <row r="22" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="5">
         <v>11</v>
       </c>
@@ -1781,28 +1963,31 @@
         <v>21</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E22" s="6"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="K22"/>
-      <c r="L22" t="s">
-        <v>99</v>
-      </c>
-      <c r="M22"/>
-    </row>
-    <row r="23" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>144</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>150</v>
+      </c>
+      <c r="F22" s="6"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="L22"/>
+      <c r="M22" t="s">
+        <v>92</v>
+      </c>
+      <c r="N22"/>
+    </row>
+    <row r="23" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A23" s="5">
         <v>11</v>
       </c>
@@ -1810,30 +1995,32 @@
         <v>22</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>149</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="I23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="K23"/>
-      <c r="L23" t="s">
-        <v>107</v>
-      </c>
-      <c r="M23"/>
-    </row>
-    <row r="24" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="J23" s="5"/>
+      <c r="K23" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="L23"/>
+      <c r="M23" t="s">
+        <v>97</v>
+      </c>
+      <c r="N23"/>
+    </row>
+    <row r="24" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A24" s="5">
         <v>12</v>
       </c>
@@ -1841,26 +2028,29 @@
         <v>23</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="K24"/>
-      <c r="L24" t="s">
-        <v>107</v>
-      </c>
-      <c r="M24"/>
-    </row>
-    <row r="25" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>142</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="L24"/>
+      <c r="M24" t="s">
+        <v>97</v>
+      </c>
+      <c r="N24"/>
+    </row>
+    <row r="25" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A25" s="5">
         <v>12</v>
       </c>
@@ -1868,28 +2058,31 @@
         <v>24</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E25" s="6"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="H25" s="5"/>
       <c r="I25" s="5"/>
-      <c r="J25" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K25"/>
-      <c r="L25" t="s">
-        <v>107</v>
-      </c>
-      <c r="M25"/>
-    </row>
-    <row r="26" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="J25" s="5"/>
+      <c r="K25" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="L25"/>
+      <c r="M25" t="s">
+        <v>97</v>
+      </c>
+      <c r="N25"/>
+    </row>
+    <row r="26" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A26" s="5">
         <v>13</v>
       </c>
@@ -1897,26 +2090,27 @@
         <v>25</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="6"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="5"/>
-      <c r="J26" s="9"/>
-      <c r="K26"/>
-      <c r="L26" t="s">
-        <v>100</v>
-      </c>
-      <c r="M26"/>
-    </row>
-    <row r="27" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="J26" s="5"/>
+      <c r="K26" s="9"/>
+      <c r="L26"/>
+      <c r="M26" t="s">
+        <v>93</v>
+      </c>
+      <c r="N26"/>
+    </row>
+    <row r="27" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A27" s="5">
         <v>13</v>
       </c>
@@ -1924,26 +2118,29 @@
         <v>26</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="8"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27"/>
-      <c r="L27" t="s">
-        <v>100</v>
-      </c>
-      <c r="M27"/>
-    </row>
-    <row r="28" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K27" s="5"/>
+      <c r="L27"/>
+      <c r="M27" t="s">
+        <v>93</v>
+      </c>
+      <c r="N27"/>
+    </row>
+    <row r="28" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A28" s="5">
         <v>14</v>
       </c>
@@ -1951,24 +2148,29 @@
         <v>27</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E28" s="6"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="5"/>
+        <v>46</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="F28" s="6"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="8"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="K28"/>
-      <c r="L28" t="s">
-        <v>100</v>
-      </c>
-      <c r="M28"/>
-    </row>
-    <row r="29" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K28" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="L28"/>
+      <c r="M28" t="s">
+        <v>93</v>
+      </c>
+      <c r="N28"/>
+    </row>
+    <row r="29" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A29" s="5">
         <v>14</v>
       </c>
@@ -1976,26 +2178,31 @@
         <v>28</v>
       </c>
       <c r="C29" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="J29" s="5"/>
+      <c r="K29" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="E29" s="6"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29"/>
-      <c r="L29" t="s">
-        <v>100</v>
-      </c>
-      <c r="M29"/>
-    </row>
-    <row r="30" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="L29"/>
+      <c r="M29" t="s">
+        <v>93</v>
+      </c>
+      <c r="N29"/>
+    </row>
+    <row r="30" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A30" s="5">
         <v>15</v>
       </c>
@@ -2003,24 +2210,25 @@
         <v>29</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="E30" s="14"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="8"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30"/>
-      <c r="L30" t="s">
-        <v>102</v>
-      </c>
-      <c r="M30"/>
-    </row>
-    <row r="31" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K30" s="5"/>
+      <c r="L30"/>
+      <c r="M30" t="s">
+        <v>94</v>
+      </c>
+      <c r="N30"/>
+    </row>
+    <row r="31" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A31" s="5">
         <v>15</v>
       </c>
@@ -2028,93 +2236,107 @@
         <v>30</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E31" s="6"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="14"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31"/>
-      <c r="L31" t="s">
-        <v>102</v>
-      </c>
-      <c r="M31"/>
-    </row>
-    <row r="32" spans="1:13">
+      <c r="K31" s="5"/>
+      <c r="L31"/>
+      <c r="M31" t="s">
+        <v>94</v>
+      </c>
+      <c r="N31"/>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" s="9"/>
       <c r="B32" s="9">
         <v>31</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E32" s="6"/>
-      <c r="F32" s="9"/>
+        <v>50</v>
+      </c>
+      <c r="E32" s="14"/>
+      <c r="F32" s="6"/>
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
-      <c r="L32" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="33" spans="4:10">
-      <c r="D33" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="34" spans="4:10">
-      <c r="D34" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="J34" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="35" spans="4:10">
-      <c r="D35" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="36" spans="4:10">
-      <c r="J36" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="37" spans="4:10">
-      <c r="J37" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="38" spans="4:10">
-      <c r="J38" s="1" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="4:10">
-      <c r="J39" s="1" t="s">
-        <v>145</v>
+      <c r="K32" s="9"/>
+      <c r="M32" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="4:11">
+      <c r="D33" s="6"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="4:11">
+      <c r="E34" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="4:11">
+      <c r="E35" s="15"/>
+    </row>
+    <row r="36" spans="4:11">
+      <c r="E36" s="15"/>
+      <c r="K36" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37" spans="4:11">
+      <c r="E37" s="15"/>
+      <c r="K37" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="4:11">
+      <c r="E38" s="15"/>
+      <c r="K38" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="4:11">
+      <c r="E39" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="4:11">
+      <c r="E40" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.5" right="0.5" top="0.5" bottom="0.5" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
syllabus changes to homework and top matter
</commit_message>
<xml_diff>
--- a/syllabus/330-syllabus.xlsx
+++ b/syllabus/330-syllabus.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25220" windowHeight="28360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="147">
   <si>
     <t>Lecture</t>
   </si>
@@ -51,12 +51,6 @@
     <t>Choose topic</t>
   </si>
   <si>
-    <t>Project proposal</t>
-  </si>
-  <si>
-    <t>Proposal feedback</t>
-  </si>
-  <si>
     <t>First draft</t>
   </si>
   <si>
@@ -87,12 +81,6 @@
     <t>Homework 5</t>
   </si>
   <si>
-    <t>Homework Reflection 4</t>
-  </si>
-  <si>
-    <t>Homework Reflection 5</t>
-  </si>
-  <si>
     <t>Outline</t>
   </si>
   <si>
@@ -160,15 +148,6 @@
   </si>
   <si>
     <t>Global Energy Policy</t>
-  </si>
-  <si>
-    <t>Homework Reflection 1</t>
-  </si>
-  <si>
-    <t>Homework Reflection 2</t>
-  </si>
-  <si>
-    <t>Homework Reflection 3</t>
   </si>
   <si>
     <t>Wrapup</t>
@@ -557,8 +536,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="165">
+  <cellStyleXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -766,7 +753,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="165">
+  <cellStyles count="173">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -849,6 +836,10 @@
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -931,6 +922,10 @@
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1265,8 +1260,8 @@
   </sheetPr>
   <dimension ref="A1:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1303,13 +1298,13 @@
         <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>4</v>
@@ -1322,10 +1317,10 @@
       </c>
       <c r="L1"/>
       <c r="M1" s="10" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="N1" s="10" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
@@ -1336,10 +1331,10 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="6"/>
@@ -1349,7 +1344,7 @@
       <c r="J2" s="5"/>
       <c r="L2"/>
       <c r="M2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="N2"/>
     </row>
@@ -1361,31 +1356,31 @@
         <v>2</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="J3" s="5"/>
       <c r="K3" s="9" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="L3"/>
       <c r="M3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
@@ -1396,13 +1391,13 @@
         <v>3</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -1410,17 +1405,17 @@
         <v>8</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="L4"/>
       <c r="M4" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
@@ -1431,26 +1426,26 @@
         <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="G5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="9" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="L5"/>
       <c r="M5" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="N5"/>
     </row>
@@ -1462,26 +1457,26 @@
         <v>5</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="9" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="L6"/>
       <c r="M6" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="N6"/>
     </row>
@@ -1493,31 +1488,31 @@
         <v>6</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="5" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="K7" s="9" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="L7"/>
       <c r="M7" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="N7"/>
     </row>
@@ -1529,13 +1524,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="5"/>
@@ -1545,11 +1540,11 @@
       </c>
       <c r="J8" s="5"/>
       <c r="K8" s="5" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="L8"/>
       <c r="M8" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="N8" s="11"/>
     </row>
@@ -1561,29 +1556,27 @@
         <v>8</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="E9" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>105</v>
-      </c>
       <c r="G9" s="5"/>
-      <c r="H9" s="5" t="s">
-        <v>47</v>
-      </c>
+      <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="9" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="L9"/>
       <c r="M9" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="N9"/>
     </row>
@@ -1595,32 +1588,32 @@
         <v>9</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="8"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="L10"/>
       <c r="M10" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="N10" s="9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
@@ -1631,26 +1624,24 @@
         <v>10</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>10</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="L11"/>
       <c r="M11" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="N11"/>
     </row>
@@ -1662,16 +1653,16 @@
         <v>11</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
@@ -1679,7 +1670,7 @@
       <c r="J12" s="5"/>
       <c r="L12"/>
       <c r="M12" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="N12" s="9"/>
     </row>
@@ -1691,26 +1682,26 @@
         <v>12</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I13" s="7"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="J13" s="5" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="L13"/>
       <c r="M13" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="N13" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
@@ -1721,26 +1712,24 @@
         <v>13</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
-      <c r="I14" s="5" t="s">
-        <v>11</v>
-      </c>
+      <c r="I14" s="5"/>
       <c r="J14" s="5"/>
       <c r="K14" s="9" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="L14"/>
       <c r="M14" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="N14"/>
     </row>
@@ -1752,23 +1741,25 @@
         <v>14</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="7"/>
+      <c r="I15" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="J15" s="5"/>
       <c r="K15" s="9"/>
       <c r="L15"/>
       <c r="M15" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="N15"/>
     </row>
@@ -1780,26 +1771,26 @@
         <v>15</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="L16"/>
       <c r="M16" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="N16"/>
     </row>
@@ -1811,26 +1802,23 @@
         <v>16</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
-      <c r="I17" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="J17" s="5"/>
       <c r="L17" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="M17" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="N17"/>
     </row>
@@ -1842,25 +1830,23 @@
         <v>17</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="6"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="5" t="s">
-        <v>49</v>
-      </c>
+      <c r="H18" s="5"/>
       <c r="I18" s="7"/>
       <c r="J18" s="5"/>
       <c r="K18" s="9"/>
       <c r="L18" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="M18" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="N18"/>
     </row>
@@ -1872,22 +1858,22 @@
         <v>18</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="K19" s="9"/>
       <c r="L19"/>
       <c r="M19" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="N19"/>
     </row>
@@ -1899,29 +1885,26 @@
         <v>19</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E20" s="14"/>
       <c r="F20" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="J20" s="5"/>
       <c r="K20" s="9" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="L20"/>
       <c r="M20" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="N20"/>
     </row>
@@ -1933,13 +1916,13 @@
         <v>20</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="5"/>
@@ -1947,11 +1930,11 @@
       <c r="I21" s="7"/>
       <c r="J21" s="5"/>
       <c r="K21" s="9" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="L21"/>
       <c r="M21" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="N21"/>
     </row>
@@ -1963,27 +1946,29 @@
         <v>21</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="5"/>
       <c r="H22" s="8"/>
-      <c r="I22" s="5"/>
+      <c r="I22" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="J22" s="5" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="K22" s="9" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="L22"/>
       <c r="M22" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="N22"/>
     </row>
@@ -1995,28 +1980,23 @@
         <v>22</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="G23" s="5"/>
-      <c r="H23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I23" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="H23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="9" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="L23"/>
       <c r="M23" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="N23"/>
     </row>
@@ -2028,25 +2008,27 @@
         <v>23</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="5"/>
       <c r="H24" s="8"/>
-      <c r="I24" s="7"/>
+      <c r="I24" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="J24" s="5"/>
       <c r="K24" s="9" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="L24"/>
       <c r="M24" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="N24"/>
     </row>
@@ -2058,27 +2040,27 @@
         <v>24</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="5"/>
       <c r="H25" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="9" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="L25"/>
       <c r="M25" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="N25"/>
     </row>
@@ -2090,23 +2072,20 @@
         <v>25</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E26" s="14"/>
       <c r="F26" s="6"/>
       <c r="G26" s="5"/>
       <c r="H26" s="8"/>
-      <c r="I26" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="J26" s="5"/>
       <c r="K26" s="9"/>
       <c r="L26"/>
       <c r="M26" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="N26"/>
     </row>
@@ -2118,16 +2097,16 @@
         <v>26</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="8"/>
@@ -2136,7 +2115,7 @@
       <c r="K27" s="5"/>
       <c r="L27"/>
       <c r="M27" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="N27"/>
     </row>
@@ -2148,13 +2127,13 @@
         <v>27</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="5"/>
@@ -2162,11 +2141,11 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
       <c r="K28" s="5" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="L28"/>
       <c r="M28" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="N28"/>
     </row>
@@ -2178,27 +2157,27 @@
         <v>28</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
       <c r="I29" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J29" s="5"/>
       <c r="K29" s="9" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="L29"/>
       <c r="M29" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="N29"/>
     </row>
@@ -2210,10 +2189,10 @@
         <v>29</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="6"/>
@@ -2224,7 +2203,7 @@
       <c r="K30" s="5"/>
       <c r="L30"/>
       <c r="M30" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="N30"/>
     </row>
@@ -2236,23 +2215,21 @@
         <v>30</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="6"/>
       <c r="G31" s="5"/>
-      <c r="H31" s="5" t="s">
-        <v>23</v>
-      </c>
+      <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
       <c r="K31" s="5"/>
       <c r="L31"/>
       <c r="M31" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="N31"/>
     </row>
@@ -2262,10 +2239,10 @@
         <v>31</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="6"/>
@@ -2275,25 +2252,25 @@
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
       <c r="M32" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="33" spans="4:11">
       <c r="D33" s="6"/>
       <c r="E33" s="15"/>
       <c r="F33" s="6" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="4:11">
       <c r="E34" s="15" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="4:11">
@@ -2302,35 +2279,35 @@
     <row r="36" spans="4:11">
       <c r="E36" s="15"/>
       <c r="K36" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="4:11">
       <c r="E37" s="15"/>
       <c r="K37" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="4:11">
       <c r="E38" s="15"/>
       <c r="K38" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="39" spans="4:11">
       <c r="E39" s="15" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="4:11">
       <c r="E40" s="15" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
syllabus ready for first class
</commit_message>
<xml_diff>
--- a/syllabus/330-syllabus.xlsx
+++ b/syllabus/330-syllabus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25220" windowHeight="28360" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="46120" windowHeight="28360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="139">
   <si>
     <t>Lecture</t>
   </si>
@@ -255,12 +255,6 @@
     <t>Lovins 1976</t>
   </si>
   <si>
-    <t>Toolkit 1</t>
-  </si>
-  <si>
-    <t>Toolkit 2</t>
-  </si>
-  <si>
     <t>HK-12 Electricity from Solar, Wind, and Hydro</t>
   </si>
   <si>
@@ -288,9 +282,6 @@
     <t>HK-13 The Building Blocks of Matter, HK-14 Nuclear Power Fission, Moore 2005</t>
   </si>
   <si>
-    <t>fracking?</t>
-  </si>
-  <si>
     <t>Impacts and Intersections</t>
   </si>
   <si>
@@ -369,21 +360,9 @@
     <t>Moore</t>
   </si>
   <si>
-    <t>check all H&amp;K readings</t>
-  </si>
-  <si>
-    <t>check all Hot Air</t>
-  </si>
-  <si>
-    <t>check all Natural Capital</t>
-  </si>
-  <si>
     <t>Check all Masters and Randolph</t>
   </si>
   <si>
-    <t>Wedges, safe operating space?</t>
-  </si>
-  <si>
     <t>GMC Sustainability Day</t>
   </si>
   <si>
@@ -396,12 +375,6 @@
     <t>Mackay-07 Heating and Cooling</t>
   </si>
   <si>
-    <t>Mackay-01, HK-01-Introduction, HK-02-Energy Mechanics</t>
-  </si>
-  <si>
-    <t>HK-03-Conservation of Energy, HK-04-Heat and Work</t>
-  </si>
-  <si>
     <t>HK-07 Energy from Fossil Fuels</t>
   </si>
   <si>
@@ -414,15 +387,6 @@
     <t>HK-19 A National and Personal Commitment</t>
   </si>
   <si>
-    <t>NC-11 Aqueous Solutions</t>
-  </si>
-  <si>
-    <t>NC-12 Climate</t>
-  </si>
-  <si>
-    <t>NC-14 Human Capitalism</t>
-  </si>
-  <si>
     <t>Energy and Water</t>
   </si>
   <si>
@@ -460,6 +424,18 @@
   </si>
   <si>
     <t>Power Africa Report, Goldemberg 1985</t>
+  </si>
+  <si>
+    <t>Mackay-01, HK-01-Introduction</t>
+  </si>
+  <si>
+    <t>Toolkit 1, HK-02-Energy Mechanics</t>
+  </si>
+  <si>
+    <t>HK-04-Heat and Work</t>
+  </si>
+  <si>
+    <t>Toolkit 2, HK-03-Conservation of Energy</t>
   </si>
 </sst>
 </file>
@@ -527,7 +503,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -535,8 +511,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="173">
+  <cellStyleXfs count="183">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -710,8 +695,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -752,8 +747,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="173">
+  <cellStyles count="183">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -840,6 +838,11 @@
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -926,6 +929,11 @@
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1258,10 +1266,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1276,12 +1284,11 @@
     <col min="8" max="8" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="65.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" ht="18" customHeight="1">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -1298,7 +1305,7 @@
         <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>3</v>
@@ -1312,18 +1319,15 @@
       <c r="J1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="L1"/>
+      <c r="K1"/>
+      <c r="L1" s="10" t="s">
+        <v>79</v>
+      </c>
       <c r="M1" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="10" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1342,13 +1346,13 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
-      <c r="L2"/>
-      <c r="M2" t="s">
-        <v>82</v>
-      </c>
-      <c r="N2"/>
-    </row>
-    <row r="3" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K2"/>
+      <c r="L2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M2"/>
+    </row>
+    <row r="3" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1362,28 +1366,22 @@
         <v>23</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G3" s="5"/>
-      <c r="H3" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="J3" s="5"/>
-      <c r="K3" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="L3"/>
-      <c r="M3" t="s">
-        <v>82</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K3"/>
+      <c r="L3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -1397,28 +1395,27 @@
         <v>24</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>78</v>
+        <v>136</v>
       </c>
       <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
+      <c r="H4" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="I4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="L4"/>
-      <c r="M4" t="s">
-        <v>82</v>
-      </c>
-      <c r="N4" s="9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>101</v>
+      </c>
+      <c r="K4"/>
+      <c r="L4" t="s">
+        <v>80</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -1432,24 +1429,21 @@
         <v>25</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>79</v>
+        <v>138</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="L5"/>
-      <c r="M5" t="s">
-        <v>82</v>
-      </c>
-      <c r="N5"/>
-    </row>
-    <row r="6" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K5"/>
+      <c r="L5" t="s">
+        <v>80</v>
+      </c>
+      <c r="M5"/>
+    </row>
+    <row r="6" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A6" s="5">
         <v>3</v>
       </c>
@@ -1462,25 +1456,22 @@
       <c r="D6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>126</v>
+      <c r="E6" s="16" t="s">
+        <v>137</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="L6"/>
-      <c r="M6" t="s">
-        <v>82</v>
-      </c>
-      <c r="N6"/>
-    </row>
-    <row r="7" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K6"/>
+      <c r="L6" t="s">
+        <v>80</v>
+      </c>
+      <c r="M6"/>
+    </row>
+    <row r="7" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A7" s="5">
         <v>3</v>
       </c>
@@ -1491,32 +1482,26 @@
         <v>50</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="G7" s="5"/>
-      <c r="H7" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="I7" s="7"/>
       <c r="J7" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="L7"/>
-      <c r="M7" t="s">
-        <v>82</v>
-      </c>
-      <c r="N7"/>
-    </row>
-    <row r="8" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>102</v>
+      </c>
+      <c r="K7"/>
+      <c r="L7" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7"/>
+    </row>
+    <row r="8" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A8" s="5">
         <v>4</v>
       </c>
@@ -1530,25 +1515,24 @@
         <v>27</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
+      <c r="H8" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="I8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="J8" s="5"/>
-      <c r="K8" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="L8"/>
-      <c r="M8" t="s">
-        <v>83</v>
-      </c>
-      <c r="N8" s="11"/>
-    </row>
-    <row r="9" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K8"/>
+      <c r="L8" t="s">
+        <v>81</v>
+      </c>
+      <c r="M8" s="11"/>
+    </row>
+    <row r="9" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A9" s="5">
         <v>4</v>
       </c>
@@ -1559,28 +1543,25 @@
         <v>52</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-      <c r="K9" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="L9"/>
-      <c r="M9" t="s">
-        <v>83</v>
-      </c>
-      <c r="N9"/>
-    </row>
-    <row r="10" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K9"/>
+      <c r="L9" t="s">
+        <v>81</v>
+      </c>
+      <c r="M9"/>
+    </row>
+    <row r="10" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A10" s="5">
         <v>5</v>
       </c>
@@ -1591,32 +1572,29 @@
         <v>53</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E10" s="14" t="s">
         <v>77</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="8"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="L10"/>
-      <c r="M10" t="s">
-        <v>83</v>
-      </c>
-      <c r="N10" s="9" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>103</v>
+      </c>
+      <c r="K10"/>
+      <c r="L10" t="s">
+        <v>81</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A11" s="5">
         <v>5</v>
       </c>
@@ -1630,22 +1608,19 @@
         <v>28</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F11" s="6"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="5" t="s">
-        <v>16</v>
-      </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-      <c r="L11"/>
-      <c r="M11" t="s">
-        <v>83</v>
-      </c>
-      <c r="N11"/>
-    </row>
-    <row r="12" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K11"/>
+      <c r="L11" t="s">
+        <v>81</v>
+      </c>
+      <c r="M11"/>
+    </row>
+    <row r="12" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A12" s="5">
         <v>6</v>
       </c>
@@ -1659,22 +1634,24 @@
         <v>29</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
+      <c r="H12" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-      <c r="L12"/>
-      <c r="M12" t="s">
-        <v>83</v>
-      </c>
-      <c r="N12" s="9"/>
-    </row>
-    <row r="13" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K12"/>
+      <c r="L12" t="s">
+        <v>81</v>
+      </c>
+      <c r="M12" s="9"/>
+    </row>
+    <row r="13" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A13" s="5">
         <v>6</v>
       </c>
@@ -1694,17 +1671,17 @@
         <v>20</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="L13"/>
+        <v>104</v>
+      </c>
+      <c r="K13"/>
+      <c r="L13" t="s">
+        <v>81</v>
+      </c>
       <c r="M13" t="s">
-        <v>83</v>
-      </c>
-      <c r="N13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A14" s="5">
         <v>7</v>
       </c>
@@ -1718,22 +1695,19 @@
         <v>31</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="L14"/>
-      <c r="M14" t="s">
-        <v>83</v>
-      </c>
-      <c r="N14"/>
-    </row>
-    <row r="15" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K14"/>
+      <c r="L14" t="s">
+        <v>81</v>
+      </c>
+      <c r="M14"/>
+    </row>
+    <row r="15" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A15" s="5">
         <v>7</v>
       </c>
@@ -1747,7 +1721,7 @@
         <v>32</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="5"/>
@@ -1756,14 +1730,13 @@
         <v>21</v>
       </c>
       <c r="J15" s="5"/>
-      <c r="K15" s="9"/>
-      <c r="L15"/>
-      <c r="M15" t="s">
-        <v>84</v>
-      </c>
-      <c r="N15"/>
-    </row>
-    <row r="16" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K15"/>
+      <c r="L15" t="s">
+        <v>82</v>
+      </c>
+      <c r="M15"/>
+    </row>
+    <row r="16" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A16" s="5">
         <v>8</v>
       </c>
@@ -1783,18 +1756,15 @@
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>138</v>
-      </c>
-      <c r="L16"/>
-      <c r="M16" t="s">
-        <v>84</v>
-      </c>
-      <c r="N16"/>
-    </row>
-    <row r="17" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>105</v>
+      </c>
+      <c r="K16"/>
+      <c r="L16" t="s">
+        <v>82</v>
+      </c>
+      <c r="M16"/>
+    </row>
+    <row r="17" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A17" s="5">
         <v>8</v>
       </c>
@@ -1808,21 +1778,21 @@
         <v>34</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="J17" s="5"/>
+      <c r="K17" t="s">
+        <v>76</v>
+      </c>
       <c r="L17" t="s">
-        <v>76</v>
-      </c>
-      <c r="M17" t="s">
-        <v>84</v>
-      </c>
-      <c r="N17"/>
-    </row>
-    <row r="18" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>82</v>
+      </c>
+      <c r="M17"/>
+    </row>
+    <row r="18" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A18" s="5">
         <v>9</v>
       </c>
@@ -1841,16 +1811,15 @@
       <c r="H18" s="5"/>
       <c r="I18" s="7"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="9"/>
+      <c r="K18" t="s">
+        <v>76</v>
+      </c>
       <c r="L18" t="s">
-        <v>76</v>
-      </c>
-      <c r="M18" t="s">
-        <v>84</v>
-      </c>
-      <c r="N18"/>
-    </row>
-    <row r="19" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>82</v>
+      </c>
+      <c r="M18"/>
+    </row>
+    <row r="19" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A19" s="5">
         <v>9</v>
       </c>
@@ -1868,16 +1837,15 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="K19" s="9"/>
-      <c r="L19"/>
-      <c r="M19" t="s">
-        <v>84</v>
-      </c>
-      <c r="N19"/>
-    </row>
-    <row r="20" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>106</v>
+      </c>
+      <c r="K19"/>
+      <c r="L19" t="s">
+        <v>82</v>
+      </c>
+      <c r="M19"/>
+    </row>
+    <row r="20" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A20" s="5">
         <v>10</v>
       </c>
@@ -1892,23 +1860,17 @@
       </c>
       <c r="E20" s="14"/>
       <c r="F20" s="6" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="G20" s="5"/>
-      <c r="H20" s="5" t="s">
-        <v>18</v>
-      </c>
       <c r="J20" s="5"/>
-      <c r="K20" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="L20"/>
-      <c r="M20" t="s">
-        <v>85</v>
-      </c>
-      <c r="N20"/>
-    </row>
-    <row r="21" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K20"/>
+      <c r="L20" t="s">
+        <v>83</v>
+      </c>
+      <c r="M20"/>
+    </row>
+    <row r="21" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A21" s="5">
         <v>10</v>
       </c>
@@ -1922,23 +1884,20 @@
         <v>38</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="7"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="L21"/>
-      <c r="M21" t="s">
-        <v>85</v>
-      </c>
-      <c r="N21"/>
-    </row>
-    <row r="22" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K21"/>
+      <c r="L21" t="s">
+        <v>83</v>
+      </c>
+      <c r="M21"/>
+    </row>
+    <row r="22" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A22" s="5">
         <v>11</v>
       </c>
@@ -1949,30 +1908,29 @@
         <v>65</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="5"/>
-      <c r="H22" s="8"/>
+      <c r="H22" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="I22" s="5" t="s">
         <v>10</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="K22" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="L22"/>
-      <c r="M22" t="s">
-        <v>85</v>
-      </c>
-      <c r="N22"/>
-    </row>
-    <row r="23" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+        <v>107</v>
+      </c>
+      <c r="K22"/>
+      <c r="L22" t="s">
+        <v>83</v>
+      </c>
+      <c r="M22"/>
+    </row>
+    <row r="23" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A23" s="5">
         <v>11</v>
       </c>
@@ -1983,24 +1941,21 @@
         <v>66</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="G23" s="5"/>
       <c r="H23" s="5"/>
       <c r="J23" s="5"/>
-      <c r="K23" s="9" t="s">
-        <v>133</v>
-      </c>
-      <c r="L23"/>
-      <c r="M23" t="s">
-        <v>90</v>
-      </c>
-      <c r="N23"/>
-    </row>
-    <row r="24" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K23"/>
+      <c r="L23" t="s">
+        <v>87</v>
+      </c>
+      <c r="M23"/>
+    </row>
+    <row r="24" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A24" s="5">
         <v>12</v>
       </c>
@@ -2011,10 +1966,10 @@
         <v>67</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="5"/>
@@ -2023,16 +1978,13 @@
         <v>11</v>
       </c>
       <c r="J24" s="5"/>
-      <c r="K24" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="L24"/>
-      <c r="M24" t="s">
-        <v>90</v>
-      </c>
-      <c r="N24"/>
-    </row>
-    <row r="25" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K24"/>
+      <c r="L24" t="s">
+        <v>87</v>
+      </c>
+      <c r="M24"/>
+    </row>
+    <row r="25" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A25" s="5">
         <v>12</v>
       </c>
@@ -2043,28 +1995,22 @@
         <v>68</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="9" t="s">
-        <v>120</v>
-      </c>
-      <c r="L25"/>
-      <c r="M25" t="s">
-        <v>90</v>
-      </c>
-      <c r="N25"/>
-    </row>
-    <row r="26" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K25"/>
+      <c r="L25" t="s">
+        <v>87</v>
+      </c>
+      <c r="M25"/>
+    </row>
+    <row r="26" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A26" s="5">
         <v>13</v>
       </c>
@@ -2080,16 +2026,17 @@
       <c r="E26" s="14"/>
       <c r="F26" s="6"/>
       <c r="G26" s="5"/>
-      <c r="H26" s="8"/>
+      <c r="H26" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="J26" s="5"/>
-      <c r="K26" s="9"/>
-      <c r="L26"/>
-      <c r="M26" t="s">
-        <v>86</v>
-      </c>
-      <c r="N26"/>
-    </row>
-    <row r="27" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K26"/>
+      <c r="L26" t="s">
+        <v>84</v>
+      </c>
+      <c r="M26"/>
+    </row>
+    <row r="27" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A27" s="5">
         <v>13</v>
       </c>
@@ -2103,23 +2050,22 @@
         <v>41</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G27" s="5"/>
       <c r="H27" s="8"/>
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27"/>
-      <c r="M27" t="s">
-        <v>86</v>
-      </c>
-      <c r="N27"/>
-    </row>
-    <row r="28" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K27"/>
+      <c r="L27" t="s">
+        <v>84</v>
+      </c>
+      <c r="M27"/>
+    </row>
+    <row r="28" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A28" s="5">
         <v>14</v>
       </c>
@@ -2133,23 +2079,20 @@
         <v>42</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="5"/>
       <c r="H28" s="8"/>
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="L28"/>
-      <c r="M28" t="s">
-        <v>86</v>
-      </c>
-      <c r="N28"/>
-    </row>
-    <row r="29" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K28"/>
+      <c r="L28" t="s">
+        <v>84</v>
+      </c>
+      <c r="M28"/>
+    </row>
+    <row r="29" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A29" s="5">
         <v>14</v>
       </c>
@@ -2163,7 +2106,7 @@
         <v>39</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="F29" s="6"/>
       <c r="G29" s="5"/>
@@ -2172,16 +2115,13 @@
         <v>12</v>
       </c>
       <c r="J29" s="5"/>
-      <c r="K29" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="L29"/>
-      <c r="M29" t="s">
-        <v>86</v>
-      </c>
-      <c r="N29"/>
-    </row>
-    <row r="30" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K29"/>
+      <c r="L29" t="s">
+        <v>84</v>
+      </c>
+      <c r="M29"/>
+    </row>
+    <row r="30" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A30" s="5">
         <v>15</v>
       </c>
@@ -2200,14 +2140,13 @@
       <c r="H30" s="8"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30"/>
-      <c r="M30" t="s">
-        <v>87</v>
-      </c>
-      <c r="N30"/>
-    </row>
-    <row r="31" spans="1:14" s="3" customFormat="1" ht="18" customHeight="1">
+      <c r="K30"/>
+      <c r="L30" t="s">
+        <v>85</v>
+      </c>
+      <c r="M30"/>
+    </row>
+    <row r="31" spans="1:13" s="3" customFormat="1" ht="18" customHeight="1">
       <c r="A31" s="5">
         <v>15</v>
       </c>
@@ -2226,14 +2165,13 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31"/>
-      <c r="M31" t="s">
-        <v>87</v>
-      </c>
-      <c r="N31"/>
-    </row>
-    <row r="32" spans="1:14">
+      <c r="K31"/>
+      <c r="L31" t="s">
+        <v>85</v>
+      </c>
+      <c r="M31"/>
+    </row>
+    <row r="32" spans="1:13">
       <c r="A32" s="9"/>
       <c r="B32" s="9">
         <v>31</v>
@@ -2250,64 +2188,45 @@
       <c r="H32" s="9"/>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="M32" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="4:11">
+      <c r="L32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6">
       <c r="D33" s="6"/>
       <c r="E33" s="15"/>
       <c r="F33" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="34" spans="4:11">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6">
       <c r="E34" s="15" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="4:11">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6">
       <c r="E35" s="15"/>
     </row>
-    <row r="36" spans="4:11">
+    <row r="36" spans="4:6">
       <c r="E36" s="15"/>
-      <c r="K36" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="37" spans="4:11">
+    </row>
+    <row r="37" spans="4:6">
       <c r="E37" s="15"/>
-      <c r="K37" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="4:11">
+    </row>
+    <row r="38" spans="4:6">
       <c r="E38" s="15"/>
-      <c r="K38" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="39" spans="4:11">
+    </row>
+    <row r="39" spans="4:6">
       <c r="E39" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="4:11">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6">
       <c r="E40" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moves reading dates, pushes back outline feedback
</commit_message>
<xml_diff>
--- a/syllabus/330-syllabus.xlsx
+++ b/syllabus/330-syllabus.xlsx
@@ -480,7 +480,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -490,6 +490,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,7 +546,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="193">
+  <cellStyleXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -734,8 +740,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -811,8 +823,22 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="193">
+  <cellStyles count="199">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -909,6 +935,9 @@
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1005,6 +1034,9 @@
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1339,8 +1371,8 @@
   </sheetPr>
   <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1674,18 +1706,18 @@
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A13" s="15">
+      <c r="A13" s="23">
         <v>12</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19" t="s">
+      <c r="D13" s="28"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G13" s="6"/>
@@ -1701,18 +1733,18 @@
       </c>
     </row>
     <row r="14" spans="1:11" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A14" s="15">
+      <c r="A14" s="31">
         <v>13</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="35"/>
       <c r="G14" s="6" t="s">
         <v>83</v>
       </c>
@@ -1724,22 +1756,18 @@
       <c r="K14"/>
     </row>
     <row r="15" spans="1:11" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A15" s="15">
+      <c r="A15" s="31">
         <v>14</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="E15" s="18"/>
-      <c r="F15" s="19" t="s">
-        <v>19</v>
-      </c>
+      <c r="D15" s="36"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="36"/>
       <c r="G15" s="6"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
@@ -1749,20 +1777,22 @@
       <c r="K15"/>
     </row>
     <row r="16" spans="1:11" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A16" s="15">
+      <c r="A16" s="31">
         <v>15</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="18" t="s">
+      <c r="D16" s="34" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="19"/>
+      <c r="F16" s="35"/>
       <c r="G16" s="6"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5" t="s">
@@ -1774,20 +1804,20 @@
       <c r="K16"/>
     </row>
     <row r="17" spans="1:11" s="3" customFormat="1" ht="18" customHeight="1">
-      <c r="A17" s="15">
+      <c r="A17" s="31">
         <v>16</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="E17" s="18"/>
-      <c r="F17" s="21"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="35" t="s">
+        <v>19</v>
+      </c>
       <c r="G17" s="6"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
@@ -1806,7 +1836,9 @@
       <c r="C18" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="18"/>
+      <c r="D18" s="18" t="s">
+        <v>119</v>
+      </c>
       <c r="E18" s="18"/>
       <c r="F18" s="22"/>
       <c r="G18" s="6"/>

</xml_diff>